<commit_message>
load characters from tables
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/Characters/enemy.xlsx
+++ b/GameConfigs/Datas/Characters/enemy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ModularSurvivor\GameConfigs\Datas\Characters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\ModularSurvivor\GameConfigs\Datas\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F655E2-EAED-4A03-AD94-44B28A553AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BD3B9B-3645-4313-8370-4B1D1C8D4737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>##var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>测试精英敌人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prefab_asset_key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level:Characters:ActorDragon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -192,7 +204,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -208,7 +220,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -524,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F925149D-7F94-4491-8C3C-719644955913}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -536,9 +548,10 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="18.25" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,8 +570,11 @@
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -577,8 +593,11 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -597,8 +616,11 @@
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -614,8 +636,11 @@
       <c r="F4">
         <v>2</v>
       </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -630,6 +655,9 @@
       </c>
       <c r="F5">
         <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add actor view Editor
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/Characters/enemy.xlsx
+++ b/GameConfigs/Datas/Characters/enemy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\ModularSurvivor\GameConfigs\Datas\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BD3B9B-3645-4313-8370-4B1D1C8D4737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F41F5-7959-4AE1-83A1-461B0CC13E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yitong Hu</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{F4D96121-8B39-42F0-91F9-0EBAF8EBD740}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yitong Hu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hero
+Enemy</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>##var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,6 +166,22 @@
   </si>
   <si>
     <t>Level:Characters:ActorDragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unit.GroupType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -138,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +204,19 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -535,11 +599,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F925149D-7F94-4491-8C3C-719644955913}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F925149D-7F94-4491-8C3C-719644955913}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -548,10 +612,11 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="18.25" customWidth="1"/>
-    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,16 +630,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -588,16 +656,19 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -611,16 +682,19 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -630,17 +704,20 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -650,18 +727,22 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5">
         <v>20</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
load character data form table
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/Characters/enemy.xlsx
+++ b/GameConfigs/Datas/Characters/enemy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\ModularSurvivor\GameConfigs\Datas\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F41F5-7959-4AE1-83A1-461B0CC13E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB919FE8-8DFC-47D8-8E4B-64E795133A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
+    <workbookView xWindow="37755" yWindow="6855" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>##var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -165,10 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Level:Characters:ActorDragon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -182,6 +178,30 @@
   </si>
   <si>
     <t>Enemy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move_speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础移动速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StraightChase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level:Characters:ActorSlime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,23 +620,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F925149D-7F94-4491-8C3C-719644955913}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="18.25" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="37.75" customWidth="1"/>
+    <col min="5" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,19 +650,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -656,19 +682,25 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -682,19 +714,25 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -705,19 +743,25 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
-        <v>23</v>
+      <c r="J4" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -728,16 +772,22 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
+      <c r="J5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apply ability to hero by table
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/Characters/enemy.xlsx
+++ b/GameConfigs/Datas/Characters/enemy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\ModularSurvivor\GameConfigs\Datas\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB919FE8-8DFC-47D8-8E4B-64E795133A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AB593D-D758-42A5-8C27-14CE37B4F89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37755" yWindow="6855" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
+    <workbookView xWindow="2565" yWindow="5055" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>##var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>Level:Characters:ActorSlime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abilities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ability config key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(array#sep=,),string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -620,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F925149D-7F94-4491-8C3C-719644955913}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -634,9 +646,10 @@
     <col min="8" max="8" width="18.25" customWidth="1"/>
     <col min="9" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="37.75" customWidth="1"/>
+    <col min="11" max="11" width="35.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,8 +680,11 @@
       <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -699,8 +715,11 @@
       <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -731,8 +750,11 @@
       <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -761,7 +783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Add AbilityConfigHitOnCollision and integrate with enemy characters; update asset catalog and manifest
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/Characters/enemy.xlsx
+++ b/GameConfigs/Datas/Characters/enemy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\ModularSurvivor\GameConfigs\Datas\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AB593D-D758-42A5-8C27-14CE37B4F89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7701CF05-0B88-41EF-A8B9-E7639B834727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="5055" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
+    <workbookView xWindow="6015" yWindow="3855" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>##var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,6 +214,13 @@
   </si>
   <si>
     <t>(array#sep=,),string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level:ActorConfigs:AbilityConfigHitOnCollision</t>
+  </si>
+  <si>
+    <t>Level:ActorConfigs:AbilityConfigHitOnCollision</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -635,7 +642,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -646,7 +653,7 @@
     <col min="8" max="8" width="18.25" customWidth="1"/>
     <col min="9" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="37.75" customWidth="1"/>
-    <col min="11" max="11" width="35.875" customWidth="1"/>
+    <col min="11" max="11" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -782,6 +789,9 @@
       <c r="J4" t="s">
         <v>32</v>
       </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -810,6 +820,9 @@
       </c>
       <c r="J5" t="s">
         <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add AbilityConfigChaseHero and integrate with enemy characters; update asset catalog and manifest
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/Characters/enemy.xlsx
+++ b/GameConfigs/Datas/Characters/enemy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\ModularSurvivor\GameConfigs\Datas\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7701CF05-0B88-41EF-A8B9-E7639B834727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E1AFF7-8CC8-4BB7-A7CB-B7FAE44BAEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6015" yWindow="3855" windowWidth="28800" windowHeight="15345" xr2:uid="{65D75327-87D2-43B9-9515-7EEF86814E57}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>##var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,10 +217,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Level:ActorConfigs:AbilityConfigHitOnCollision</t>
-  </si>
-  <si>
-    <t>Level:ActorConfigs:AbilityConfigHitOnCollision</t>
+    <t>Level:ActorConfigs:AbilityConfigHitOnCollision,Level:ActorConfigs:AbilityConfigChaseHero</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -790,7 +787,7 @@
         <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>